<commit_message>
create two large-scale problem
</commit_message>
<xml_diff>
--- a/large/record.xlsx
+++ b/large/record.xlsx
@@ -5,15 +5,16 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/canli/euler/hierarchy/large/3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/canli/euler/hierarchy/large/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="3 s" sheetId="2" r:id="rId2"/>
+    <sheet name="9s" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="69">
   <si>
     <t xml:space="preserve"> 801.243]</t>
   </si>
@@ -184,6 +185,54 @@
   </si>
   <si>
     <t>LB</t>
+  </si>
+  <si>
+    <t>178828 Any</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 735       .531</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 781.       39</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 79       1.676</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 795.0       78</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8       00.68</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 806.861]</t>
+  </si>
+  <si>
+    <t>178829 Any</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9       95.102</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 952.40       5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 820.       362</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 104       2.84</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 835.22       3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 858       .441</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1       036.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 806.947]</t>
   </si>
 </sst>
 </file>
@@ -6616,7 +6665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GO7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -7842,4 +7891,2829 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:GS203"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="K183" sqref="K183"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:201" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>468.87200000000001</v>
+      </c>
+      <c r="E1">
+        <v>472.55799999999999</v>
+      </c>
+      <c r="F1">
+        <v>477.94099999999997</v>
+      </c>
+      <c r="G1">
+        <v>511.279</v>
+      </c>
+      <c r="H1">
+        <v>530.73400000000004</v>
+      </c>
+      <c r="I1">
+        <v>533.49599999999998</v>
+      </c>
+      <c r="J1">
+        <v>545.45100000000002</v>
+      </c>
+      <c r="K1">
+        <v>557.85699999999997</v>
+      </c>
+      <c r="L1">
+        <v>562.07000000000005</v>
+      </c>
+      <c r="M1">
+        <v>586.51400000000001</v>
+      </c>
+      <c r="N1">
+        <v>594.649</v>
+      </c>
+      <c r="O1">
+        <v>607.029</v>
+      </c>
+      <c r="P1">
+        <v>612.69500000000005</v>
+      </c>
+      <c r="Q1">
+        <v>619.94299999999998</v>
+      </c>
+      <c r="R1">
+        <v>628.73400000000004</v>
+      </c>
+      <c r="S1">
+        <v>631.56899999999996</v>
+      </c>
+      <c r="T1">
+        <v>651.46900000000005</v>
+      </c>
+      <c r="U1">
+        <v>653.404</v>
+      </c>
+      <c r="V1">
+        <v>655.53099999999995</v>
+      </c>
+      <c r="W1">
+        <v>661.41399999999999</v>
+      </c>
+      <c r="X1">
+        <v>662.73199999999997</v>
+      </c>
+      <c r="Y1">
+        <v>669.70799999999997</v>
+      </c>
+      <c r="Z1">
+        <v>683.62900000000002</v>
+      </c>
+      <c r="AA1">
+        <v>684.64</v>
+      </c>
+      <c r="AB1">
+        <v>692.36599999999999</v>
+      </c>
+      <c r="AC1">
+        <v>693.14099999999996</v>
+      </c>
+      <c r="AD1">
+        <v>694.98500000000001</v>
+      </c>
+      <c r="AE1">
+        <v>696.34299999999996</v>
+      </c>
+      <c r="AF1">
+        <v>700.99099999999999</v>
+      </c>
+      <c r="AG1">
+        <v>705.80100000000004</v>
+      </c>
+      <c r="AH1">
+        <v>708.92399999999998</v>
+      </c>
+      <c r="AI1">
+        <v>709.39</v>
+      </c>
+      <c r="AJ1">
+        <v>710.51700000000005</v>
+      </c>
+      <c r="AK1">
+        <v>713.27499999999998</v>
+      </c>
+      <c r="AL1">
+        <v>717.69799999999998</v>
+      </c>
+      <c r="AM1">
+        <v>720.33799999999997</v>
+      </c>
+      <c r="AN1">
+        <v>724.88300000000004</v>
+      </c>
+      <c r="AO1">
+        <v>730.16099999999994</v>
+      </c>
+      <c r="AP1">
+        <v>734.04</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR1">
+        <v>736.66099999999994</v>
+      </c>
+      <c r="AS1">
+        <v>738.73500000000001</v>
+      </c>
+      <c r="AT1">
+        <v>739.56500000000005</v>
+      </c>
+      <c r="AU1">
+        <v>750.28300000000002</v>
+      </c>
+      <c r="AV1">
+        <v>755.98699999999997</v>
+      </c>
+      <c r="AW1">
+        <v>760.86</v>
+      </c>
+      <c r="AX1">
+        <v>762.44</v>
+      </c>
+      <c r="AY1">
+        <v>766.49599999999998</v>
+      </c>
+      <c r="AZ1">
+        <v>768.25099999999998</v>
+      </c>
+      <c r="BA1">
+        <v>768.91600000000005</v>
+      </c>
+      <c r="BB1">
+        <v>769.91399999999999</v>
+      </c>
+      <c r="BC1">
+        <v>770.63199999999995</v>
+      </c>
+      <c r="BD1">
+        <v>772.18</v>
+      </c>
+      <c r="BE1">
+        <v>772.81299999999999</v>
+      </c>
+      <c r="BF1">
+        <v>773.27499999999998</v>
+      </c>
+      <c r="BG1">
+        <v>773.41099999999994</v>
+      </c>
+      <c r="BH1">
+        <v>775.15300000000002</v>
+      </c>
+      <c r="BI1">
+        <v>775.29200000000003</v>
+      </c>
+      <c r="BJ1">
+        <v>775.625</v>
+      </c>
+      <c r="BK1">
+        <v>776.84699999999998</v>
+      </c>
+      <c r="BL1">
+        <v>776.95</v>
+      </c>
+      <c r="BM1">
+        <v>778.46199999999999</v>
+      </c>
+      <c r="BN1">
+        <v>778.61400000000003</v>
+      </c>
+      <c r="BO1">
+        <v>778.846</v>
+      </c>
+      <c r="BP1">
+        <v>779.11400000000003</v>
+      </c>
+      <c r="BQ1">
+        <v>779.34</v>
+      </c>
+      <c r="BR1">
+        <v>779.524</v>
+      </c>
+      <c r="BS1">
+        <v>779.91</v>
+      </c>
+      <c r="BT1">
+        <v>780.22299999999996</v>
+      </c>
+      <c r="BU1">
+        <v>780.38400000000001</v>
+      </c>
+      <c r="BV1">
+        <v>780.48599999999999</v>
+      </c>
+      <c r="BW1">
+        <v>780.69100000000003</v>
+      </c>
+      <c r="BX1">
+        <v>780.86800000000005</v>
+      </c>
+      <c r="BY1">
+        <v>780.93600000000004</v>
+      </c>
+      <c r="BZ1">
+        <v>781.02300000000002</v>
+      </c>
+      <c r="CA1">
+        <v>781.06799999999998</v>
+      </c>
+      <c r="CB1">
+        <v>781.07899999999995</v>
+      </c>
+      <c r="CC1">
+        <v>781.09100000000001</v>
+      </c>
+      <c r="CD1">
+        <v>781.10799999999995</v>
+      </c>
+      <c r="CE1">
+        <v>781.10799999999995</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>55</v>
+      </c>
+      <c r="CG1">
+        <v>781.61400000000003</v>
+      </c>
+      <c r="CH1">
+        <v>781.83199999999999</v>
+      </c>
+      <c r="CI1">
+        <v>781.83799999999997</v>
+      </c>
+      <c r="CJ1">
+        <v>782.06899999999996</v>
+      </c>
+      <c r="CK1">
+        <v>782.07</v>
+      </c>
+      <c r="CL1">
+        <v>782.072</v>
+      </c>
+      <c r="CM1">
+        <v>782.07299999999998</v>
+      </c>
+      <c r="CN1">
+        <v>782.21900000000005</v>
+      </c>
+      <c r="CO1">
+        <v>782.22299999999996</v>
+      </c>
+      <c r="CP1">
+        <v>782.95299999999997</v>
+      </c>
+      <c r="CQ1">
+        <v>783.30399999999997</v>
+      </c>
+      <c r="CR1">
+        <v>783.30499999999995</v>
+      </c>
+      <c r="CS1">
+        <v>783.68799999999999</v>
+      </c>
+      <c r="CT1">
+        <v>785.71799999999996</v>
+      </c>
+      <c r="CU1">
+        <v>785.74300000000005</v>
+      </c>
+      <c r="CV1">
+        <v>786.21400000000006</v>
+      </c>
+      <c r="CW1">
+        <v>786.25599999999997</v>
+      </c>
+      <c r="CX1">
+        <v>786.26499999999999</v>
+      </c>
+      <c r="CY1">
+        <v>786.28099999999995</v>
+      </c>
+      <c r="CZ1">
+        <v>786.37699999999995</v>
+      </c>
+      <c r="DA1">
+        <v>786.38599999999997</v>
+      </c>
+      <c r="DB1">
+        <v>786.45899999999995</v>
+      </c>
+      <c r="DC1">
+        <v>786.45899999999995</v>
+      </c>
+      <c r="DD1">
+        <v>786.91800000000001</v>
+      </c>
+      <c r="DE1">
+        <v>787.58</v>
+      </c>
+      <c r="DF1">
+        <v>787.58299999999997</v>
+      </c>
+      <c r="DG1">
+        <v>787.61199999999997</v>
+      </c>
+      <c r="DH1">
+        <v>787.65300000000002</v>
+      </c>
+      <c r="DI1">
+        <v>787.65899999999999</v>
+      </c>
+      <c r="DJ1">
+        <v>788.64099999999996</v>
+      </c>
+      <c r="DK1">
+        <v>788.64400000000001</v>
+      </c>
+      <c r="DL1">
+        <v>788.66399999999999</v>
+      </c>
+      <c r="DM1">
+        <v>788.66800000000001</v>
+      </c>
+      <c r="DN1">
+        <v>789.904</v>
+      </c>
+      <c r="DO1">
+        <v>789.904</v>
+      </c>
+      <c r="DP1">
+        <v>790.34299999999996</v>
+      </c>
+      <c r="DQ1">
+        <v>790.46299999999997</v>
+      </c>
+      <c r="DR1">
+        <v>790.47199999999998</v>
+      </c>
+      <c r="DS1">
+        <v>791.19600000000003</v>
+      </c>
+      <c r="DT1">
+        <v>791.21299999999997</v>
+      </c>
+      <c r="DU1" t="s">
+        <v>56</v>
+      </c>
+      <c r="DV1">
+        <v>792.08699999999999</v>
+      </c>
+      <c r="DW1">
+        <v>792.15899999999999</v>
+      </c>
+      <c r="DX1">
+        <v>792.38400000000001</v>
+      </c>
+      <c r="DY1">
+        <v>792.38900000000001</v>
+      </c>
+      <c r="DZ1">
+        <v>792.53499999999997</v>
+      </c>
+      <c r="EA1">
+        <v>792.54600000000005</v>
+      </c>
+      <c r="EB1">
+        <v>792.55100000000004</v>
+      </c>
+      <c r="EC1">
+        <v>792.56500000000005</v>
+      </c>
+      <c r="ED1">
+        <v>792.65300000000002</v>
+      </c>
+      <c r="EE1">
+        <v>792.78300000000002</v>
+      </c>
+      <c r="EF1">
+        <v>793.06600000000003</v>
+      </c>
+      <c r="EG1">
+        <v>793.08600000000001</v>
+      </c>
+      <c r="EH1">
+        <v>793.73699999999997</v>
+      </c>
+      <c r="EI1">
+        <v>793.73900000000003</v>
+      </c>
+      <c r="EJ1">
+        <v>793.74800000000005</v>
+      </c>
+      <c r="EK1">
+        <v>793.88599999999997</v>
+      </c>
+      <c r="EL1">
+        <v>794.02599999999995</v>
+      </c>
+      <c r="EM1">
+        <v>794.05600000000004</v>
+      </c>
+      <c r="EN1">
+        <v>794.13</v>
+      </c>
+      <c r="EO1" t="s">
+        <v>57</v>
+      </c>
+      <c r="EP1">
+        <v>795.08900000000006</v>
+      </c>
+      <c r="EQ1">
+        <v>795.77</v>
+      </c>
+      <c r="ER1">
+        <v>796.05600000000004</v>
+      </c>
+      <c r="ES1">
+        <v>796.06</v>
+      </c>
+      <c r="ET1">
+        <v>796.81700000000001</v>
+      </c>
+      <c r="EU1">
+        <v>797.798</v>
+      </c>
+      <c r="EV1">
+        <v>797.80399999999997</v>
+      </c>
+      <c r="EW1">
+        <v>797.82299999999998</v>
+      </c>
+      <c r="EX1">
+        <v>797.84199999999998</v>
+      </c>
+      <c r="EY1">
+        <v>797.84699999999998</v>
+      </c>
+      <c r="EZ1">
+        <v>797.87699999999995</v>
+      </c>
+      <c r="FA1">
+        <v>797.88199999999995</v>
+      </c>
+      <c r="FB1">
+        <v>797.98800000000006</v>
+      </c>
+      <c r="FC1">
+        <v>797.98900000000003</v>
+      </c>
+      <c r="FD1">
+        <v>798.17100000000005</v>
+      </c>
+      <c r="FE1">
+        <v>798.63099999999997</v>
+      </c>
+      <c r="FF1">
+        <v>798.63099999999997</v>
+      </c>
+      <c r="FG1">
+        <v>798.63499999999999</v>
+      </c>
+      <c r="FH1">
+        <v>799.00800000000004</v>
+      </c>
+      <c r="FI1">
+        <v>799.84</v>
+      </c>
+      <c r="FJ1" t="s">
+        <v>58</v>
+      </c>
+      <c r="FK1">
+        <v>801.64400000000001</v>
+      </c>
+      <c r="FL1">
+        <v>801.755</v>
+      </c>
+      <c r="FM1">
+        <v>801.89599999999996</v>
+      </c>
+      <c r="FN1">
+        <v>802.04</v>
+      </c>
+      <c r="FO1">
+        <v>802.04</v>
+      </c>
+      <c r="FP1">
+        <v>802.48500000000001</v>
+      </c>
+      <c r="FQ1">
+        <v>802.50900000000001</v>
+      </c>
+      <c r="FR1">
+        <v>802.84500000000003</v>
+      </c>
+      <c r="FS1">
+        <v>803.24400000000003</v>
+      </c>
+      <c r="FT1">
+        <v>803.58399999999995</v>
+      </c>
+      <c r="FU1">
+        <v>803.76900000000001</v>
+      </c>
+      <c r="FV1">
+        <v>803.81100000000004</v>
+      </c>
+      <c r="FW1">
+        <v>803.899</v>
+      </c>
+      <c r="FX1">
+        <v>804.01400000000001</v>
+      </c>
+      <c r="FY1">
+        <v>804.05700000000002</v>
+      </c>
+      <c r="FZ1">
+        <v>804.54700000000003</v>
+      </c>
+      <c r="GA1">
+        <v>804.66</v>
+      </c>
+      <c r="GB1">
+        <v>804.66099999999994</v>
+      </c>
+      <c r="GC1">
+        <v>805.09</v>
+      </c>
+      <c r="GD1">
+        <v>805.12099999999998</v>
+      </c>
+      <c r="GE1">
+        <v>805.53399999999999</v>
+      </c>
+      <c r="GF1">
+        <v>805.53599999999994</v>
+      </c>
+      <c r="GG1">
+        <v>805.56500000000005</v>
+      </c>
+      <c r="GH1">
+        <v>805.65499999999997</v>
+      </c>
+      <c r="GI1">
+        <v>805.74599999999998</v>
+      </c>
+      <c r="GJ1">
+        <v>805.83600000000001</v>
+      </c>
+      <c r="GK1">
+        <v>806.51</v>
+      </c>
+      <c r="GL1">
+        <v>806.55600000000004</v>
+      </c>
+      <c r="GM1">
+        <v>806.56700000000001</v>
+      </c>
+      <c r="GN1">
+        <v>806.65300000000002</v>
+      </c>
+      <c r="GO1">
+        <v>806.65300000000002</v>
+      </c>
+      <c r="GP1">
+        <v>806.774</v>
+      </c>
+      <c r="GQ1">
+        <v>806.84199999999998</v>
+      </c>
+      <c r="GR1">
+        <v>806.84900000000005</v>
+      </c>
+      <c r="GS1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:201" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2">
+        <v>1325</v>
+      </c>
+      <c r="C2">
+        <v>1052.54</v>
+      </c>
+      <c r="D2">
+        <v>1049.0999999999999</v>
+      </c>
+      <c r="E2">
+        <v>1027.96</v>
+      </c>
+      <c r="F2">
+        <v>1222.03</v>
+      </c>
+      <c r="G2">
+        <v>1220.8</v>
+      </c>
+      <c r="H2">
+        <v>1404.74</v>
+      </c>
+      <c r="I2">
+        <v>1333.39</v>
+      </c>
+      <c r="J2">
+        <v>1123.6099999999999</v>
+      </c>
+      <c r="K2">
+        <v>1081.6500000000001</v>
+      </c>
+      <c r="L2">
+        <v>1066.1600000000001</v>
+      </c>
+      <c r="M2">
+        <v>989.17600000000004</v>
+      </c>
+      <c r="N2">
+        <v>1033.1099999999999</v>
+      </c>
+      <c r="O2">
+        <v>1033.6199999999999</v>
+      </c>
+      <c r="P2">
+        <v>912.64700000000005</v>
+      </c>
+      <c r="Q2">
+        <v>1141.42</v>
+      </c>
+      <c r="R2">
+        <v>902.95299999999997</v>
+      </c>
+      <c r="S2">
+        <v>873.93200000000002</v>
+      </c>
+      <c r="T2">
+        <v>854.37400000000002</v>
+      </c>
+      <c r="U2">
+        <v>893.94299999999998</v>
+      </c>
+      <c r="V2" t="s">
+        <v>61</v>
+      </c>
+      <c r="W2">
+        <v>885.73</v>
+      </c>
+      <c r="X2">
+        <v>931.64499999999998</v>
+      </c>
+      <c r="Y2">
+        <v>854.13099999999997</v>
+      </c>
+      <c r="Z2">
+        <v>872.78300000000002</v>
+      </c>
+      <c r="AA2">
+        <v>822.28599999999994</v>
+      </c>
+      <c r="AB2">
+        <v>826.75199999999995</v>
+      </c>
+      <c r="AC2">
+        <v>841.76599999999996</v>
+      </c>
+      <c r="AD2">
+        <v>853.88599999999997</v>
+      </c>
+      <c r="AE2">
+        <v>977.399</v>
+      </c>
+      <c r="AF2">
+        <v>847.52599999999995</v>
+      </c>
+      <c r="AG2">
+        <v>1157.8</v>
+      </c>
+      <c r="AH2">
+        <v>1026.81</v>
+      </c>
+      <c r="AI2">
+        <v>873.39700000000005</v>
+      </c>
+      <c r="AJ2">
+        <v>838.57</v>
+      </c>
+      <c r="AK2">
+        <v>838.04700000000003</v>
+      </c>
+      <c r="AL2">
+        <v>836.62099999999998</v>
+      </c>
+      <c r="AM2">
+        <v>999.20699999999999</v>
+      </c>
+      <c r="AN2">
+        <v>830.755</v>
+      </c>
+      <c r="AO2">
+        <v>909.61599999999999</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ2">
+        <v>1073.79</v>
+      </c>
+      <c r="AR2">
+        <v>862.62300000000005</v>
+      </c>
+      <c r="AS2">
+        <v>1020.55</v>
+      </c>
+      <c r="AT2">
+        <v>828.94299999999998</v>
+      </c>
+      <c r="AU2">
+        <v>884.25800000000004</v>
+      </c>
+      <c r="AV2">
+        <v>822.46199999999999</v>
+      </c>
+      <c r="AW2">
+        <v>798.8</v>
+      </c>
+      <c r="AX2">
+        <v>850.67</v>
+      </c>
+      <c r="AY2">
+        <v>844.32899999999995</v>
+      </c>
+      <c r="AZ2">
+        <v>832.11900000000003</v>
+      </c>
+      <c r="BA2">
+        <v>952.08199999999999</v>
+      </c>
+      <c r="BB2">
+        <v>809.53899999999999</v>
+      </c>
+      <c r="BC2">
+        <v>792.82799999999997</v>
+      </c>
+      <c r="BD2">
+        <v>964.40099999999995</v>
+      </c>
+      <c r="BE2">
+        <v>812.28</v>
+      </c>
+      <c r="BF2">
+        <v>812.85900000000004</v>
+      </c>
+      <c r="BG2">
+        <v>856.52099999999996</v>
+      </c>
+      <c r="BH2">
+        <v>1088.2</v>
+      </c>
+      <c r="BI2">
+        <v>950.95699999999999</v>
+      </c>
+      <c r="BJ2">
+        <v>790.62599999999998</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BL2">
+        <v>818.04600000000005</v>
+      </c>
+      <c r="BM2">
+        <v>860.02099999999996</v>
+      </c>
+      <c r="BN2">
+        <v>788.73099999999999</v>
+      </c>
+      <c r="BO2">
+        <v>821.61</v>
+      </c>
+      <c r="BP2">
+        <v>811.47699999999998</v>
+      </c>
+      <c r="BQ2">
+        <v>787.78499999999997</v>
+      </c>
+      <c r="BR2">
+        <v>844.322</v>
+      </c>
+      <c r="BS2">
+        <v>783.26</v>
+      </c>
+      <c r="BT2">
+        <v>877.56399999999996</v>
+      </c>
+      <c r="BU2">
+        <v>811.23400000000004</v>
+      </c>
+      <c r="BV2">
+        <v>781.745</v>
+      </c>
+      <c r="BW2">
+        <v>781.83100000000002</v>
+      </c>
+      <c r="BX2">
+        <v>781.39499999999998</v>
+      </c>
+      <c r="BY2">
+        <v>781.25699999999995</v>
+      </c>
+      <c r="BZ2">
+        <v>781.2</v>
+      </c>
+      <c r="CA2">
+        <v>781.17</v>
+      </c>
+      <c r="CB2">
+        <v>781.17</v>
+      </c>
+      <c r="CC2">
+        <v>807.27599999999995</v>
+      </c>
+      <c r="CD2">
+        <v>832.44200000000001</v>
+      </c>
+      <c r="CE2">
+        <v>832.41200000000003</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>64</v>
+      </c>
+      <c r="CG2">
+        <v>833.91800000000001</v>
+      </c>
+      <c r="CH2">
+        <v>1043.25</v>
+      </c>
+      <c r="CI2">
+        <v>859.40099999999995</v>
+      </c>
+      <c r="CJ2">
+        <v>831.74099999999999</v>
+      </c>
+      <c r="CK2">
+        <v>831.71100000000001</v>
+      </c>
+      <c r="CL2">
+        <v>831.71699999999998</v>
+      </c>
+      <c r="CM2">
+        <v>831.69399999999996</v>
+      </c>
+      <c r="CN2">
+        <v>897.697</v>
+      </c>
+      <c r="CO2">
+        <v>897.73500000000001</v>
+      </c>
+      <c r="CP2">
+        <v>831.29899999999998</v>
+      </c>
+      <c r="CQ2">
+        <v>830.27599999999995</v>
+      </c>
+      <c r="CR2">
+        <v>830.202</v>
+      </c>
+      <c r="CS2">
+        <v>831.577</v>
+      </c>
+      <c r="CT2">
+        <v>870.59</v>
+      </c>
+      <c r="CU2">
+        <v>870.58199999999999</v>
+      </c>
+      <c r="CV2">
+        <v>873.58699999999999</v>
+      </c>
+      <c r="CW2">
+        <v>862.28200000000004</v>
+      </c>
+      <c r="CX2">
+        <v>862.24599999999998</v>
+      </c>
+      <c r="CY2">
+        <v>873.59199999999998</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>65</v>
+      </c>
+      <c r="DA2">
+        <v>835.21600000000001</v>
+      </c>
+      <c r="DB2">
+        <v>825.18600000000004</v>
+      </c>
+      <c r="DC2">
+        <v>825.16</v>
+      </c>
+      <c r="DD2">
+        <v>830.24900000000002</v>
+      </c>
+      <c r="DE2">
+        <v>986.23400000000004</v>
+      </c>
+      <c r="DF2">
+        <v>986.07600000000002</v>
+      </c>
+      <c r="DG2">
+        <v>986.06399999999996</v>
+      </c>
+      <c r="DH2">
+        <v>872.26499999999999</v>
+      </c>
+      <c r="DI2">
+        <v>872.19899999999996</v>
+      </c>
+      <c r="DJ2">
+        <v>1026.99</v>
+      </c>
+      <c r="DK2">
+        <v>1026.92</v>
+      </c>
+      <c r="DL2">
+        <v>1026.68</v>
+      </c>
+      <c r="DM2">
+        <v>1026.6199999999999</v>
+      </c>
+      <c r="DN2">
+        <v>905.11199999999997</v>
+      </c>
+      <c r="DO2">
+        <v>905.00699999999995</v>
+      </c>
+      <c r="DP2">
+        <v>1009.07</v>
+      </c>
+      <c r="DQ2">
+        <v>843.96699999999998</v>
+      </c>
+      <c r="DR2">
+        <v>843.93799999999999</v>
+      </c>
+      <c r="DS2">
+        <v>925.60799999999995</v>
+      </c>
+      <c r="DT2">
+        <v>925.62199999999996</v>
+      </c>
+      <c r="DU2">
+        <v>863.95100000000002</v>
+      </c>
+      <c r="DV2">
+        <v>1052.6099999999999</v>
+      </c>
+      <c r="DW2">
+        <v>843.26400000000001</v>
+      </c>
+      <c r="DX2">
+        <v>884.93</v>
+      </c>
+      <c r="DY2">
+        <v>884.928</v>
+      </c>
+      <c r="DZ2">
+        <v>1004.71</v>
+      </c>
+      <c r="EA2">
+        <v>1052.8900000000001</v>
+      </c>
+      <c r="EB2">
+        <v>1004.63</v>
+      </c>
+      <c r="EC2">
+        <v>1004.58</v>
+      </c>
+      <c r="ED2">
+        <v>1004.59</v>
+      </c>
+      <c r="EE2">
+        <v>828.25199999999995</v>
+      </c>
+      <c r="EF2">
+        <v>1003.91</v>
+      </c>
+      <c r="EG2">
+        <v>1003.82</v>
+      </c>
+      <c r="EH2">
+        <v>1053.9100000000001</v>
+      </c>
+      <c r="EI2">
+        <v>850.15200000000004</v>
+      </c>
+      <c r="EJ2">
+        <v>850.11800000000005</v>
+      </c>
+      <c r="EK2">
+        <v>849.53499999999997</v>
+      </c>
+      <c r="EL2">
+        <v>909.60400000000004</v>
+      </c>
+      <c r="EM2">
+        <v>909.54300000000001</v>
+      </c>
+      <c r="EN2">
+        <v>1054.06</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>66</v>
+      </c>
+      <c r="EP2">
+        <v>858.37599999999998</v>
+      </c>
+      <c r="EQ2">
+        <v>855.81399999999996</v>
+      </c>
+      <c r="ER2">
+        <v>830.63499999999999</v>
+      </c>
+      <c r="ES2">
+        <v>830.62400000000002</v>
+      </c>
+      <c r="ET2">
+        <v>857.72900000000004</v>
+      </c>
+      <c r="EU2">
+        <v>1031.2</v>
+      </c>
+      <c r="EV2">
+        <v>1031.06</v>
+      </c>
+      <c r="EW2">
+        <v>1031.0999999999999</v>
+      </c>
+      <c r="EX2">
+        <v>1030.24</v>
+      </c>
+      <c r="EY2">
+        <v>1030.0899999999999</v>
+      </c>
+      <c r="EZ2">
+        <v>1030.1300000000001</v>
+      </c>
+      <c r="FA2">
+        <v>1029.98</v>
+      </c>
+      <c r="FB2">
+        <v>842.18499999999995</v>
+      </c>
+      <c r="FC2">
+        <v>842.17200000000003</v>
+      </c>
+      <c r="FD2">
+        <v>838.59</v>
+      </c>
+      <c r="FE2">
+        <v>842.87099999999998</v>
+      </c>
+      <c r="FF2">
+        <v>842.83799999999997</v>
+      </c>
+      <c r="FG2">
+        <v>842.83900000000006</v>
+      </c>
+      <c r="FH2">
+        <v>819.90800000000002</v>
+      </c>
+      <c r="FI2">
+        <v>847.44600000000003</v>
+      </c>
+      <c r="FJ2">
+        <v>829.423</v>
+      </c>
+      <c r="FK2">
+        <v>1052.17</v>
+      </c>
+      <c r="FL2">
+        <v>822.22799999999995</v>
+      </c>
+      <c r="FM2">
+        <v>1051.93</v>
+      </c>
+      <c r="FN2">
+        <v>832.00800000000004</v>
+      </c>
+      <c r="FO2">
+        <v>831.97799999999995</v>
+      </c>
+      <c r="FP2">
+        <v>887.78200000000004</v>
+      </c>
+      <c r="FQ2">
+        <v>887.56200000000001</v>
+      </c>
+      <c r="FR2">
+        <v>840.745</v>
+      </c>
+      <c r="FS2">
+        <v>836.20799999999997</v>
+      </c>
+      <c r="FT2">
+        <v>819.07100000000003</v>
+      </c>
+      <c r="FU2">
+        <v>1031.1199999999999</v>
+      </c>
+      <c r="FV2">
+        <v>1031.07</v>
+      </c>
+      <c r="FW2">
+        <v>831.02099999999996</v>
+      </c>
+      <c r="FX2">
+        <v>1031.4100000000001</v>
+      </c>
+      <c r="FY2">
+        <v>1031.3699999999999</v>
+      </c>
+      <c r="FZ2">
+        <v>810.48299999999995</v>
+      </c>
+      <c r="GA2">
+        <v>842.90800000000002</v>
+      </c>
+      <c r="GB2">
+        <v>842.85699999999997</v>
+      </c>
+      <c r="GC2">
+        <v>811.41600000000005</v>
+      </c>
+      <c r="GD2" t="s">
+        <v>67</v>
+      </c>
+      <c r="GE2">
+        <v>846.07</v>
+      </c>
+      <c r="GF2">
+        <v>845.995</v>
+      </c>
+      <c r="GG2">
+        <v>834.71799999999996</v>
+      </c>
+      <c r="GH2">
+        <v>825.90899999999999</v>
+      </c>
+      <c r="GI2">
+        <v>807.91099999999994</v>
+      </c>
+      <c r="GJ2">
+        <v>807.55100000000004</v>
+      </c>
+      <c r="GK2">
+        <v>809.03899999999999</v>
+      </c>
+      <c r="GL2">
+        <v>878.476</v>
+      </c>
+      <c r="GM2">
+        <v>878.53800000000001</v>
+      </c>
+      <c r="GN2">
+        <v>834.17100000000005</v>
+      </c>
+      <c r="GO2">
+        <v>834.19500000000005</v>
+      </c>
+      <c r="GP2">
+        <v>807.101</v>
+      </c>
+      <c r="GQ2">
+        <v>807.00400000000002</v>
+      </c>
+      <c r="GR2">
+        <v>806.98500000000001</v>
+      </c>
+      <c r="GS2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:201" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:201" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1052.54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:201" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>468.87200000000001</v>
+      </c>
+      <c r="B6">
+        <v>1049.0999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:201" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>472.55799999999999</v>
+      </c>
+      <c r="B7">
+        <v>1027.96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:201" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>477.94099999999997</v>
+      </c>
+      <c r="B8">
+        <v>1222.03</v>
+      </c>
+    </row>
+    <row r="9" spans="1:201" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>511.279</v>
+      </c>
+      <c r="B9">
+        <v>1220.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:201" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>530.73400000000004</v>
+      </c>
+      <c r="B10">
+        <v>1404.74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:201" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>533.49599999999998</v>
+      </c>
+      <c r="B11">
+        <v>1333.39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:201" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>545.45100000000002</v>
+      </c>
+      <c r="B12">
+        <v>1123.6099999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:201" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>557.85699999999997</v>
+      </c>
+      <c r="B13">
+        <v>1081.6500000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:201" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>562.07000000000005</v>
+      </c>
+      <c r="B14">
+        <v>1066.1600000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:201" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>586.51400000000001</v>
+      </c>
+      <c r="B15">
+        <v>989.17600000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:201" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>594.649</v>
+      </c>
+      <c r="B16">
+        <v>1033.1099999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>607.029</v>
+      </c>
+      <c r="B17">
+        <v>1033.6199999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>612.69500000000005</v>
+      </c>
+      <c r="B18">
+        <v>912.64700000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>619.94299999999998</v>
+      </c>
+      <c r="B19">
+        <v>1141.42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>628.73400000000004</v>
+      </c>
+      <c r="B20">
+        <v>902.95299999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>631.56899999999996</v>
+      </c>
+      <c r="B21">
+        <v>873.93200000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>651.46900000000005</v>
+      </c>
+      <c r="B22">
+        <v>854.37400000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>653.404</v>
+      </c>
+      <c r="B23">
+        <v>893.94299999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>655.53099999999995</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>661.41399999999999</v>
+      </c>
+      <c r="B25">
+        <v>885.73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>662.73199999999997</v>
+      </c>
+      <c r="B26">
+        <v>931.64499999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>669.70799999999997</v>
+      </c>
+      <c r="B27">
+        <v>854.13099999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>683.62900000000002</v>
+      </c>
+      <c r="B28">
+        <v>872.78300000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>684.64</v>
+      </c>
+      <c r="B29">
+        <v>822.28599999999994</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>692.36599999999999</v>
+      </c>
+      <c r="B30">
+        <v>826.75199999999995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>693.14099999999996</v>
+      </c>
+      <c r="B31">
+        <v>841.76599999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>694.98500000000001</v>
+      </c>
+      <c r="B32">
+        <v>853.88599999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>696.34299999999996</v>
+      </c>
+      <c r="B33">
+        <v>977.399</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>700.99099999999999</v>
+      </c>
+      <c r="B34">
+        <v>847.52599999999995</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>705.80100000000004</v>
+      </c>
+      <c r="B35">
+        <v>1157.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>708.92399999999998</v>
+      </c>
+      <c r="B36">
+        <v>1026.81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>709.39</v>
+      </c>
+      <c r="B37">
+        <v>873.39700000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>710.51700000000005</v>
+      </c>
+      <c r="B38">
+        <v>838.57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>713.27499999999998</v>
+      </c>
+      <c r="B39">
+        <v>838.04700000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>717.69799999999998</v>
+      </c>
+      <c r="B40">
+        <v>836.62099999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>720.33799999999997</v>
+      </c>
+      <c r="B41">
+        <v>999.20699999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>724.88300000000004</v>
+      </c>
+      <c r="B42">
+        <v>830.755</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>730.16099999999994</v>
+      </c>
+      <c r="B43">
+        <v>909.61599999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>734.04</v>
+      </c>
+      <c r="B44" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45">
+        <v>1073.79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>736.66099999999994</v>
+      </c>
+      <c r="B46">
+        <v>862.62300000000005</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>738.73500000000001</v>
+      </c>
+      <c r="B47">
+        <v>1020.55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>739.56500000000005</v>
+      </c>
+      <c r="B48">
+        <v>828.94299999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>750.28300000000002</v>
+      </c>
+      <c r="B49">
+        <v>884.25800000000004</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>755.98699999999997</v>
+      </c>
+      <c r="B50">
+        <v>822.46199999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>760.86</v>
+      </c>
+      <c r="B51">
+        <v>798.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>762.44</v>
+      </c>
+      <c r="B52">
+        <v>850.67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>766.49599999999998</v>
+      </c>
+      <c r="B53">
+        <v>844.32899999999995</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>768.25099999999998</v>
+      </c>
+      <c r="B54">
+        <v>832.11900000000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>768.91600000000005</v>
+      </c>
+      <c r="B55">
+        <v>952.08199999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>769.91399999999999</v>
+      </c>
+      <c r="B56">
+        <v>809.53899999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>770.63199999999995</v>
+      </c>
+      <c r="B57">
+        <v>792.82799999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>772.18</v>
+      </c>
+      <c r="B58">
+        <v>964.40099999999995</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>772.81299999999999</v>
+      </c>
+      <c r="B59">
+        <v>812.28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>773.27499999999998</v>
+      </c>
+      <c r="B60">
+        <v>812.85900000000004</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>773.41099999999994</v>
+      </c>
+      <c r="B61">
+        <v>856.52099999999996</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>775.15300000000002</v>
+      </c>
+      <c r="B62">
+        <v>1088.2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>775.29200000000003</v>
+      </c>
+      <c r="B63">
+        <v>950.95699999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>775.625</v>
+      </c>
+      <c r="B64">
+        <v>790.62599999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>776.84699999999998</v>
+      </c>
+      <c r="B65" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>776.95</v>
+      </c>
+      <c r="B66">
+        <v>818.04600000000005</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>778.46199999999999</v>
+      </c>
+      <c r="B67">
+        <v>860.02099999999996</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>778.61400000000003</v>
+      </c>
+      <c r="B68">
+        <v>788.73099999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>778.846</v>
+      </c>
+      <c r="B69">
+        <v>821.61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>779.11400000000003</v>
+      </c>
+      <c r="B70">
+        <v>811.47699999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>779.34</v>
+      </c>
+      <c r="B71">
+        <v>787.78499999999997</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>779.524</v>
+      </c>
+      <c r="B72">
+        <v>844.322</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>779.91</v>
+      </c>
+      <c r="B73">
+        <v>783.26</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>780.22299999999996</v>
+      </c>
+      <c r="B74">
+        <v>877.56399999999996</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>780.38400000000001</v>
+      </c>
+      <c r="B75">
+        <v>811.23400000000004</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>780.48599999999999</v>
+      </c>
+      <c r="B76">
+        <v>781.745</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>780.69100000000003</v>
+      </c>
+      <c r="B77">
+        <v>781.83100000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>780.86800000000005</v>
+      </c>
+      <c r="B78">
+        <v>781.39499999999998</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>780.93600000000004</v>
+      </c>
+      <c r="B79">
+        <v>781.25699999999995</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>781.02300000000002</v>
+      </c>
+      <c r="B80">
+        <v>781.2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>781.06799999999998</v>
+      </c>
+      <c r="B81">
+        <v>781.17</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>781.07899999999995</v>
+      </c>
+      <c r="B82">
+        <v>781.17</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>781.09100000000001</v>
+      </c>
+      <c r="B83">
+        <v>807.27599999999995</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>781.10799999999995</v>
+      </c>
+      <c r="B84">
+        <v>832.44200000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>781.10799999999995</v>
+      </c>
+      <c r="B85">
+        <v>832.41200000000003</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>55</v>
+      </c>
+      <c r="B86" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>781.61400000000003</v>
+      </c>
+      <c r="B87">
+        <v>833.91800000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>781.83199999999999</v>
+      </c>
+      <c r="B88">
+        <v>1043.25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>781.83799999999997</v>
+      </c>
+      <c r="B89">
+        <v>859.40099999999995</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>782.06899999999996</v>
+      </c>
+      <c r="B90">
+        <v>831.74099999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>782.07</v>
+      </c>
+      <c r="B91">
+        <v>831.71100000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>782.072</v>
+      </c>
+      <c r="B92">
+        <v>831.71699999999998</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>782.07299999999998</v>
+      </c>
+      <c r="B93">
+        <v>831.69399999999996</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>782.21900000000005</v>
+      </c>
+      <c r="B94">
+        <v>897.697</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>782.22299999999996</v>
+      </c>
+      <c r="B95">
+        <v>897.73500000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>782.95299999999997</v>
+      </c>
+      <c r="B96">
+        <v>831.29899999999998</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>783.30399999999997</v>
+      </c>
+      <c r="B97">
+        <v>830.27599999999995</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>783.30499999999995</v>
+      </c>
+      <c r="B98">
+        <v>830.202</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>783.68799999999999</v>
+      </c>
+      <c r="B99">
+        <v>831.577</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>785.71799999999996</v>
+      </c>
+      <c r="B100">
+        <v>870.59</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>785.74300000000005</v>
+      </c>
+      <c r="B101">
+        <v>870.58199999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>786.21400000000006</v>
+      </c>
+      <c r="B102">
+        <v>873.58699999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>786.25599999999997</v>
+      </c>
+      <c r="B103">
+        <v>862.28200000000004</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>786.26499999999999</v>
+      </c>
+      <c r="B104">
+        <v>862.24599999999998</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>786.28099999999995</v>
+      </c>
+      <c r="B105">
+        <v>873.59199999999998</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>786.37699999999995</v>
+      </c>
+      <c r="B106" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>786.38599999999997</v>
+      </c>
+      <c r="B107">
+        <v>835.21600000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>786.45899999999995</v>
+      </c>
+      <c r="B108">
+        <v>825.18600000000004</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>786.45899999999995</v>
+      </c>
+      <c r="B109">
+        <v>825.16</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>786.91800000000001</v>
+      </c>
+      <c r="B110">
+        <v>830.24900000000002</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>787.58</v>
+      </c>
+      <c r="B111">
+        <v>986.23400000000004</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>787.58299999999997</v>
+      </c>
+      <c r="B112">
+        <v>986.07600000000002</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>787.61199999999997</v>
+      </c>
+      <c r="B113">
+        <v>986.06399999999996</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>787.65300000000002</v>
+      </c>
+      <c r="B114">
+        <v>872.26499999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>787.65899999999999</v>
+      </c>
+      <c r="B115">
+        <v>872.19899999999996</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>788.64099999999996</v>
+      </c>
+      <c r="B116">
+        <v>1026.99</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>788.64400000000001</v>
+      </c>
+      <c r="B117">
+        <v>1026.92</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>788.66399999999999</v>
+      </c>
+      <c r="B118">
+        <v>1026.68</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>788.66800000000001</v>
+      </c>
+      <c r="B119">
+        <v>1026.6199999999999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>789.904</v>
+      </c>
+      <c r="B120">
+        <v>905.11199999999997</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>789.904</v>
+      </c>
+      <c r="B121">
+        <v>905.00699999999995</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>790.34299999999996</v>
+      </c>
+      <c r="B122">
+        <v>1009.07</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>790.46299999999997</v>
+      </c>
+      <c r="B123">
+        <v>843.96699999999998</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>790.47199999999998</v>
+      </c>
+      <c r="B124">
+        <v>843.93799999999999</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>791.19600000000003</v>
+      </c>
+      <c r="B125">
+        <v>925.60799999999995</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>791.21299999999997</v>
+      </c>
+      <c r="B126">
+        <v>925.62199999999996</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>56</v>
+      </c>
+      <c r="B127">
+        <v>863.95100000000002</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>792.08699999999999</v>
+      </c>
+      <c r="B128">
+        <v>1052.6099999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>792.15899999999999</v>
+      </c>
+      <c r="B129">
+        <v>843.26400000000001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>792.38400000000001</v>
+      </c>
+      <c r="B130">
+        <v>884.93</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>792.38900000000001</v>
+      </c>
+      <c r="B131">
+        <v>884.928</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>792.53499999999997</v>
+      </c>
+      <c r="B132">
+        <v>1004.71</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>792.54600000000005</v>
+      </c>
+      <c r="B133">
+        <v>1052.8900000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>792.55100000000004</v>
+      </c>
+      <c r="B134">
+        <v>1004.63</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>792.56500000000005</v>
+      </c>
+      <c r="B135">
+        <v>1004.58</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>792.65300000000002</v>
+      </c>
+      <c r="B136">
+        <v>1004.59</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>792.78300000000002</v>
+      </c>
+      <c r="B137">
+        <v>828.25199999999995</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>793.06600000000003</v>
+      </c>
+      <c r="B138">
+        <v>1003.91</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>793.08600000000001</v>
+      </c>
+      <c r="B139">
+        <v>1003.82</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>793.73699999999997</v>
+      </c>
+      <c r="B140">
+        <v>1053.9100000000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>793.73900000000003</v>
+      </c>
+      <c r="B141">
+        <v>850.15200000000004</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>793.74800000000005</v>
+      </c>
+      <c r="B142">
+        <v>850.11800000000005</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>793.88599999999997</v>
+      </c>
+      <c r="B143">
+        <v>849.53499999999997</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>794.02599999999995</v>
+      </c>
+      <c r="B144">
+        <v>909.60400000000004</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>794.05600000000004</v>
+      </c>
+      <c r="B145">
+        <v>909.54300000000001</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>794.13</v>
+      </c>
+      <c r="B146">
+        <v>1054.06</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>57</v>
+      </c>
+      <c r="B147" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>795.08900000000006</v>
+      </c>
+      <c r="B148">
+        <v>858.37599999999998</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>795.77</v>
+      </c>
+      <c r="B149">
+        <v>855.81399999999996</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>796.05600000000004</v>
+      </c>
+      <c r="B150">
+        <v>830.63499999999999</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>796.06</v>
+      </c>
+      <c r="B151">
+        <v>830.62400000000002</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>796.81700000000001</v>
+      </c>
+      <c r="B152">
+        <v>857.72900000000004</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>797.798</v>
+      </c>
+      <c r="B153">
+        <v>1031.2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>797.80399999999997</v>
+      </c>
+      <c r="B154">
+        <v>1031.06</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>797.82299999999998</v>
+      </c>
+      <c r="B155">
+        <v>1031.0999999999999</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>797.84199999999998</v>
+      </c>
+      <c r="B156">
+        <v>1030.24</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>797.84699999999998</v>
+      </c>
+      <c r="B157">
+        <v>1030.0899999999999</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>797.87699999999995</v>
+      </c>
+      <c r="B158">
+        <v>1030.1300000000001</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>797.88199999999995</v>
+      </c>
+      <c r="B159">
+        <v>1029.98</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>797.98800000000006</v>
+      </c>
+      <c r="B160">
+        <v>842.18499999999995</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>797.98900000000003</v>
+      </c>
+      <c r="B161">
+        <v>842.17200000000003</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>798.17100000000005</v>
+      </c>
+      <c r="B162">
+        <v>838.59</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>798.63099999999997</v>
+      </c>
+      <c r="B163">
+        <v>842.87099999999998</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>798.63099999999997</v>
+      </c>
+      <c r="B164">
+        <v>842.83799999999997</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>798.63499999999999</v>
+      </c>
+      <c r="B165">
+        <v>842.83900000000006</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>799.00800000000004</v>
+      </c>
+      <c r="B166">
+        <v>819.90800000000002</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>799.84</v>
+      </c>
+      <c r="B167">
+        <v>847.44600000000003</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>58</v>
+      </c>
+      <c r="B168">
+        <v>829.423</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>801.64400000000001</v>
+      </c>
+      <c r="B169">
+        <v>1052.17</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>801.755</v>
+      </c>
+      <c r="B170">
+        <v>822.22799999999995</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>801.89599999999996</v>
+      </c>
+      <c r="B171">
+        <v>1051.93</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>802.04</v>
+      </c>
+      <c r="B172">
+        <v>832.00800000000004</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>802.04</v>
+      </c>
+      <c r="B173">
+        <v>831.97799999999995</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>802.48500000000001</v>
+      </c>
+      <c r="B174">
+        <v>887.78200000000004</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>802.50900000000001</v>
+      </c>
+      <c r="B175">
+        <v>887.56200000000001</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>802.84500000000003</v>
+      </c>
+      <c r="B176">
+        <v>840.745</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>803.24400000000003</v>
+      </c>
+      <c r="B177">
+        <v>836.20799999999997</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>803.58399999999995</v>
+      </c>
+      <c r="B178">
+        <v>819.07100000000003</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>803.76900000000001</v>
+      </c>
+      <c r="B179">
+        <v>1031.1199999999999</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>803.81100000000004</v>
+      </c>
+      <c r="B180">
+        <v>1031.07</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>803.899</v>
+      </c>
+      <c r="B181">
+        <v>831.02099999999996</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>804.01400000000001</v>
+      </c>
+      <c r="B182">
+        <v>1031.4100000000001</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>804.05700000000002</v>
+      </c>
+      <c r="B183">
+        <v>1031.3699999999999</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>804.54700000000003</v>
+      </c>
+      <c r="B184">
+        <v>810.48299999999995</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>804.66</v>
+      </c>
+      <c r="B185">
+        <v>842.90800000000002</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>804.66099999999994</v>
+      </c>
+      <c r="B186">
+        <v>842.85699999999997</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>805.09</v>
+      </c>
+      <c r="B187">
+        <v>811.41600000000005</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>805.12099999999998</v>
+      </c>
+      <c r="B188" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>805.53399999999999</v>
+      </c>
+      <c r="B189">
+        <v>846.07</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>805.53599999999994</v>
+      </c>
+      <c r="B190">
+        <v>845.995</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>805.56500000000005</v>
+      </c>
+      <c r="B191">
+        <v>834.71799999999996</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>805.65499999999997</v>
+      </c>
+      <c r="B192">
+        <v>825.90899999999999</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>805.74599999999998</v>
+      </c>
+      <c r="B193">
+        <v>807.91099999999994</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>805.83600000000001</v>
+      </c>
+      <c r="B194">
+        <v>807.55100000000004</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>806.51</v>
+      </c>
+      <c r="B195">
+        <v>809.03899999999999</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>806.55600000000004</v>
+      </c>
+      <c r="B196">
+        <v>878.476</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>806.56700000000001</v>
+      </c>
+      <c r="B197">
+        <v>878.53800000000001</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>806.65300000000002</v>
+      </c>
+      <c r="B198">
+        <v>834.17100000000005</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>806.65300000000002</v>
+      </c>
+      <c r="B199">
+        <v>834.19500000000005</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>806.774</v>
+      </c>
+      <c r="B200">
+        <v>807.101</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <v>806.84199999999998</v>
+      </c>
+      <c r="B201">
+        <v>807.00400000000002</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>806.84900000000005</v>
+      </c>
+      <c r="B202">
+        <v>806.98500000000001</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>59</v>
+      </c>
+      <c r="B203" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>